<commit_message>
add correct construction RPE-PR model
</commit_message>
<xml_diff>
--- a/rxn_bounds/R3D301_EX_rxns_RPE-PR.xlsx
+++ b/rxn_bounds/R3D301_EX_rxns_RPE-PR.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\prins\git\Human1_RPE-PR\rxn_bounds\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\prins\GitHub\Human1_RPE-PR\rxn_bounds\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDC55B9D-AC1F-443B-A16F-E806D436AEDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E8E94C7-2526-478D-8A27-34DD18A2505B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{69497B25-CBDB-B04B-AD57-06C30CF64D2B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{69497B25-CBDB-B04B-AD57-06C30CF64D2B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14679,106 +14679,106 @@
     <t>MAR09721_RPE</t>
   </si>
   <si>
-    <t>MAR09034_eRPE-PR</t>
-  </si>
-  <si>
-    <t>MAR09438_eRPE-PR</t>
-  </si>
-  <si>
-    <t>MAR09081_eRPE-PR</t>
-  </si>
-  <si>
-    <t>MAR00628_eRPE-PR</t>
-  </si>
-  <si>
-    <t>MAR09135_eRPE-PR</t>
-  </si>
-  <si>
-    <t>MAR09061_eRPE-PR</t>
-  </si>
-  <si>
-    <t>MAR09216_eRPE-PR</t>
-  </si>
-  <si>
-    <t>MAR09063_eRPE-PR</t>
-  </si>
-  <si>
-    <t>MAR09134_eRPE-PR</t>
-  </si>
-  <si>
-    <t>MAR09067_eRPE-PR</t>
-  </si>
-  <si>
-    <t>MAR09065_eRPE-PR</t>
-  </si>
-  <si>
-    <t>MAR09071_eRPE-PR</t>
-  </si>
-  <si>
-    <t>MAR09068_eRPE-PR</t>
-  </si>
-  <si>
-    <t>MAR09041_eRPE-PR</t>
-  </si>
-  <si>
-    <t>MAR09046_eRPE-PR</t>
-  </si>
-  <si>
-    <t>MAR09040_eRPE-PR</t>
-  </si>
-  <si>
-    <t>MAR09069_eRPE-PR</t>
-  </si>
-  <si>
-    <t>MAR09087_eRPE-PR</t>
-  </si>
-  <si>
-    <t>MAR09044_eRPE-PR</t>
-  </si>
-  <si>
-    <t>MAR09133_eRPE-PR</t>
-  </si>
-  <si>
-    <t>MAR09286_eRPE-PR</t>
-  </si>
-  <si>
-    <t>MAR09132_eRPE-PR</t>
-  </si>
-  <si>
-    <t>MAR09039_eRPE-PR</t>
-  </si>
-  <si>
-    <t>MAR09043_eRPE-PR</t>
-  </si>
-  <si>
-    <t>MAR09351_eRPE-PR</t>
-  </si>
-  <si>
-    <t>MAR09064_eRPE-PR</t>
-  </si>
-  <si>
-    <t>MAR09460_eRPE-PR</t>
-  </si>
-  <si>
-    <t>MAR09045_eRPE-PR</t>
-  </si>
-  <si>
-    <t>MAR09070_eRPE-PR</t>
-  </si>
-  <si>
-    <t>MAR09066_eRPE-PR</t>
-  </si>
-  <si>
-    <t>MAR09201_eRPE-PR</t>
-  </si>
-  <si>
-    <t>MAR09042_eRPE-PR</t>
-  </si>
-  <si>
-    <t>MAR09415_eRPE-PR</t>
-  </si>
-  <si>
-    <t>MAR09161_eRPE-PR</t>
+    <t>MAR09161_RPE-PR</t>
+  </si>
+  <si>
+    <t>MAR09415_RPE-PR</t>
+  </si>
+  <si>
+    <t>MAR09042_RPE-PR</t>
+  </si>
+  <si>
+    <t>MAR09201_RPE-PR</t>
+  </si>
+  <si>
+    <t>MAR09066_RPE-PR</t>
+  </si>
+  <si>
+    <t>MAR09070_RPE-PR</t>
+  </si>
+  <si>
+    <t>MAR09045_RPE-PR</t>
+  </si>
+  <si>
+    <t>MAR09460_RPE-PR</t>
+  </si>
+  <si>
+    <t>MAR09064_RPE-PR</t>
+  </si>
+  <si>
+    <t>MAR09351_RPE-PR</t>
+  </si>
+  <si>
+    <t>MAR09043_RPE-PR</t>
+  </si>
+  <si>
+    <t>MAR09039_RPE-PR</t>
+  </si>
+  <si>
+    <t>MAR09132_RPE-PR</t>
+  </si>
+  <si>
+    <t>MAR09286_RPE-PR</t>
+  </si>
+  <si>
+    <t>MAR09133_RPE-PR</t>
+  </si>
+  <si>
+    <t>MAR09044_RPE-PR</t>
+  </si>
+  <si>
+    <t>MAR09069_RPE-PR</t>
+  </si>
+  <si>
+    <t>MAR09087_RPE-PR</t>
+  </si>
+  <si>
+    <t>MAR09040_RPE-PR</t>
+  </si>
+  <si>
+    <t>MAR09046_RPE-PR</t>
+  </si>
+  <si>
+    <t>MAR09041_RPE-PR</t>
+  </si>
+  <si>
+    <t>MAR09034_RPE-PR</t>
+  </si>
+  <si>
+    <t>MAR09438_RPE-PR</t>
+  </si>
+  <si>
+    <t>MAR09081_RPE-PR</t>
+  </si>
+  <si>
+    <t>MAR00628_RPE-PR</t>
+  </si>
+  <si>
+    <t>MAR09135_RPE-PR</t>
+  </si>
+  <si>
+    <t>MAR09061_RPE-PR</t>
+  </si>
+  <si>
+    <t>MAR09216_RPE-PR</t>
+  </si>
+  <si>
+    <t>MAR09063_RPE-PR</t>
+  </si>
+  <si>
+    <t>MAR09134_RPE-PR</t>
+  </si>
+  <si>
+    <t>MAR09067_RPE-PR</t>
+  </si>
+  <si>
+    <t>MAR09065_RPE-PR</t>
+  </si>
+  <si>
+    <t>MAR09071_RPE-PR</t>
+  </si>
+  <si>
+    <t>MAR09068_RPE-PR</t>
   </si>
 </sst>
 </file>
@@ -15152,7 +15152,7 @@
   <dimension ref="A1:E1672"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -15186,7 +15186,7 @@
         <v>1664</v>
       </c>
       <c r="C2" t="s">
-        <v>4880</v>
+        <v>4901</v>
       </c>
       <c r="D2">
         <v>7800000</v>
@@ -15204,7 +15204,7 @@
         <v>2026</v>
       </c>
       <c r="C3" t="s">
-        <v>4881</v>
+        <v>4902</v>
       </c>
       <c r="D3">
         <v>7100000</v>
@@ -15222,7 +15222,7 @@
         <v>1706</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>4882</v>
+        <v>4903</v>
       </c>
       <c r="D4" s="4">
         <v>5000000</v>
@@ -15240,7 +15240,7 @@
         <v>2109</v>
       </c>
       <c r="C5" t="s">
-        <v>4883</v>
+        <v>4904</v>
       </c>
       <c r="D5">
         <v>1908000</v>
@@ -15258,7 +15258,7 @@
         <v>1759</v>
       </c>
       <c r="C6" t="s">
-        <v>4884</v>
+        <v>4905</v>
       </c>
       <c r="D6">
         <v>1800000</v>
@@ -15276,7 +15276,7 @@
         <v>1687</v>
       </c>
       <c r="C7" t="s">
-        <v>4885</v>
+        <v>4906</v>
       </c>
       <c r="D7">
         <v>564000</v>
@@ -15294,7 +15294,7 @@
         <v>1809</v>
       </c>
       <c r="C8" t="s">
-        <v>4886</v>
+        <v>4907</v>
       </c>
       <c r="D8">
         <v>540000</v>
@@ -15312,7 +15312,7 @@
         <v>1689</v>
       </c>
       <c r="C9" t="s">
-        <v>4887</v>
+        <v>4908</v>
       </c>
       <c r="D9">
         <v>517000</v>
@@ -15330,7 +15330,7 @@
         <v>1758</v>
       </c>
       <c r="C10" t="s">
-        <v>4888</v>
+        <v>4909</v>
       </c>
       <c r="D10">
         <v>500000</v>
@@ -15348,7 +15348,7 @@
         <v>1693</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>4889</v>
+        <v>4910</v>
       </c>
       <c r="D11" s="4">
         <v>390000</v>
@@ -15366,7 +15366,7 @@
         <v>1691</v>
       </c>
       <c r="C12" t="s">
-        <v>4890</v>
+        <v>4911</v>
       </c>
       <c r="D12">
         <v>357000</v>
@@ -15384,7 +15384,7 @@
         <v>1697</v>
       </c>
       <c r="C13" t="s">
-        <v>4891</v>
+        <v>4912</v>
       </c>
       <c r="D13">
         <v>261000</v>
@@ -15402,7 +15402,7 @@
         <v>1694</v>
       </c>
       <c r="C14" t="s">
-        <v>4892</v>
+        <v>4913</v>
       </c>
       <c r="D14">
         <v>245000</v>
@@ -15420,7 +15420,7 @@
         <v>1670</v>
       </c>
       <c r="C15" t="s">
-        <v>4893</v>
+        <v>4900</v>
       </c>
       <c r="D15">
         <v>241000</v>
@@ -15438,7 +15438,7 @@
         <v>1675</v>
       </c>
       <c r="C16" t="s">
-        <v>4894</v>
+        <v>4899</v>
       </c>
       <c r="D16">
         <v>230000</v>
@@ -15456,7 +15456,7 @@
         <v>1669</v>
       </c>
       <c r="C17" t="s">
-        <v>4895</v>
+        <v>4898</v>
       </c>
       <c r="D17">
         <v>205000</v>
@@ -15510,7 +15510,7 @@
         <v>1673</v>
       </c>
       <c r="C20" t="s">
-        <v>4898</v>
+        <v>4895</v>
       </c>
       <c r="D20">
         <v>164000</v>
@@ -15528,7 +15528,7 @@
         <v>1757</v>
       </c>
       <c r="C21" t="s">
-        <v>4899</v>
+        <v>4894</v>
       </c>
       <c r="D21">
         <v>160000</v>
@@ -15546,7 +15546,7 @@
         <v>1878</v>
       </c>
       <c r="C22" t="s">
-        <v>4900</v>
+        <v>4893</v>
       </c>
       <c r="D22">
         <v>128000</v>
@@ -15564,7 +15564,7 @@
         <v>1756</v>
       </c>
       <c r="C23" t="s">
-        <v>4901</v>
+        <v>4892</v>
       </c>
       <c r="D23">
         <v>100000</v>
@@ -15582,7 +15582,7 @@
         <v>1668</v>
       </c>
       <c r="C24" t="s">
-        <v>4902</v>
+        <v>4891</v>
       </c>
       <c r="D24">
         <v>99000</v>
@@ -15600,7 +15600,7 @@
         <v>1672</v>
       </c>
       <c r="C25" t="s">
-        <v>4903</v>
+        <v>4890</v>
       </c>
       <c r="D25">
         <v>95000</v>
@@ -15618,7 +15618,7 @@
         <v>1942</v>
       </c>
       <c r="C26" t="s">
-        <v>4904</v>
+        <v>4889</v>
       </c>
       <c r="D26">
         <v>89400</v>
@@ -15636,7 +15636,7 @@
         <v>1690</v>
       </c>
       <c r="C27" t="s">
-        <v>4905</v>
+        <v>4888</v>
       </c>
       <c r="D27">
         <v>77000</v>
@@ -15654,7 +15654,7 @@
         <v>2045</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>4906</v>
+        <v>4887</v>
       </c>
       <c r="D28" s="4">
         <v>74100</v>
@@ -15672,7 +15672,7 @@
         <v>1674</v>
       </c>
       <c r="C29" t="s">
-        <v>4907</v>
+        <v>4886</v>
       </c>
       <c r="D29">
         <v>69000</v>
@@ -15690,7 +15690,7 @@
         <v>1696</v>
       </c>
       <c r="C30" t="s">
-        <v>4908</v>
+        <v>4885</v>
       </c>
       <c r="D30">
         <v>66000</v>
@@ -15708,7 +15708,7 @@
         <v>1692</v>
       </c>
       <c r="C31" t="s">
-        <v>4909</v>
+        <v>4884</v>
       </c>
       <c r="D31">
         <v>51000</v>
@@ -15726,7 +15726,7 @@
         <v>1795</v>
       </c>
       <c r="C32" t="s">
-        <v>4910</v>
+        <v>4883</v>
       </c>
       <c r="D32">
         <v>29800</v>
@@ -15744,7 +15744,7 @@
         <v>1671</v>
       </c>
       <c r="C33" t="s">
-        <v>4911</v>
+        <v>4882</v>
       </c>
       <c r="D33">
         <v>29000</v>
@@ -15762,7 +15762,7 @@
         <v>2003</v>
       </c>
       <c r="C34" t="s">
-        <v>4912</v>
+        <v>4881</v>
       </c>
       <c r="D34">
         <v>10100</v>
@@ -15780,7 +15780,7 @@
         <v>1785</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>4913</v>
+        <v>4880</v>
       </c>
       <c r="D35" s="4">
         <v>200</v>

</xml_diff>